<commit_message>
Pantalla AdministrarPlanEstudio y Modificaciones ImportarCalificaciones
</commit_message>
<xml_diff>
--- a/src/main/webapp/recursos/plantilla_importar_alumnos.xlsx
+++ b/src/main/webapp/recursos/plantilla_importar_alumnos.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\NetBeansProjects\sistemaUniversidades_XP\src\main\webapp\recursos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hector\Desktop\GIT\Versión 4\sistemaUniversidades_XP\src\main\webapp\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A165A882-6690-4EAD-B374-5E4B85CCAAA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3255" yWindow="975" windowWidth="15375" windowHeight="9615" xr2:uid="{B2DADF52-93B2-4522-AF0D-E1CCEB769197}"/>
+    <workbookView xWindow="3255" yWindow="975" windowWidth="15375" windowHeight="9615"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,22 +24,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>101010</t>
+    <t>MATRICULA</t>
   </si>
   <si>
-    <t>Ejemplo</t>
+    <t>NOMBRE</t>
   </si>
   <si>
-    <t>CURPEJEMPLO</t>
+    <t>CURP</t>
+  </si>
+  <si>
+    <t>189625</t>
+  </si>
+  <si>
+    <t>Carlos Segoviano</t>
+  </si>
+  <si>
+    <t>SACC000117HSRLLRA5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -49,12 +57,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -77,10 +90,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,31 +412,164 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B94E487-192F-4D1A-9784-D09C13C9DA62}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="19.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>